<commit_message>
Scenarios Excel spreadsheet updated
</commit_message>
<xml_diff>
--- a/SCENARIOS.xlsx
+++ b/SCENARIOS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="25">
   <si>
     <t>COLOR</t>
   </si>
@@ -75,6 +75,30 @@
   </si>
   <si>
     <t>FRONT OF SWITCH</t>
+  </si>
+  <si>
+    <t>SIDE OF SCALE</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>FRONT OF SCALE</t>
+  </si>
+  <si>
+    <t>LEFT SIDE</t>
+  </si>
+  <si>
+    <t>RIGHT SIDE</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>CROSS LINE LEFT</t>
+  </si>
+  <si>
+    <t>CROSS LINE RIGHT</t>
   </si>
 </sst>
 </file>
@@ -98,15 +122,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -129,20 +171,372 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFF3232"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -417,190 +811,781 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G12"/>
+  <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="39.88671875" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
-    <col min="7" max="7" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="H4" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="H5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="25">
+        <v>2</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11">
+        <v>3</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="20">
+        <v>1</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="28">
+        <v>2</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="13">
+        <v>2</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="20">
+        <v>2</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="15">
+        <v>3</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="20">
+        <v>3</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>